<commit_message>
began working on coding heirarchy
</commit_message>
<xml_diff>
--- a/categorySort/notebooks/data/completedHeiarachy.xlsx
+++ b/categorySort/notebooks/data/completedHeiarachy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh\Desktop\Projects\Random\categorySort\notebooks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAEE255-80F4-4651-BF12-79424A3019C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F60C82-96FF-4666-B9C3-8D5D372F904C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2370" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12249" uniqueCount="5320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12254" uniqueCount="5322">
   <si>
     <t>Survey</t>
   </si>
@@ -15996,6 +15996,12 @@
   </si>
   <si>
     <t>Infant clothing</t>
+  </si>
+  <si>
+    <t>Code Desc</t>
+  </si>
+  <si>
+    <t>Level5</t>
   </si>
 </sst>
 </file>
@@ -16423,7 +16429,7 @@
   <dimension ref="A1:K5050"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+      <selection activeCell="G227" sqref="G227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16448,8 +16454,12 @@
         <v>5054</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5320</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5321</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -18732,7 +18742,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A209" s="2" t="s">
         <v>208</v>
       </c>
@@ -18743,7 +18753,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="210" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A210" s="2" t="s">
         <v>209</v>
       </c>
@@ -18754,7 +18764,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A211" s="2" t="s">
         <v>210</v>
       </c>
@@ -18765,7 +18775,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A212" s="2" t="s">
         <v>211</v>
       </c>
@@ -18776,7 +18786,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A213" s="2" t="s">
         <v>215</v>
       </c>
@@ -18789,8 +18799,17 @@
       <c r="D213" t="s">
         <v>5256</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+      <c r="G213" t="s">
+        <v>3791</v>
+      </c>
+      <c r="H213" t="s">
+        <v>5056</v>
+      </c>
+      <c r="I213" t="s">
+        <v>5063</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A214" s="2" t="s">
         <v>216</v>
       </c>
@@ -18801,7 +18820,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A215" s="2" t="s">
         <v>217</v>
       </c>
@@ -18815,7 +18834,7 @@
         <v>3791</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A216" s="2" t="s">
         <v>218</v>
       </c>
@@ -18829,7 +18848,7 @@
         <v>3791</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A217" s="2" t="s">
         <v>219</v>
       </c>
@@ -18843,7 +18862,7 @@
         <v>3791</v>
       </c>
     </row>
-    <row r="218" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A218" s="2" t="s">
         <v>220</v>
       </c>
@@ -18854,7 +18873,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A219" s="2" t="s">
         <v>221</v>
       </c>
@@ -18865,7 +18884,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A220" s="2" t="s">
         <v>213</v>
       </c>
@@ -18879,7 +18898,7 @@
         <v>5255</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A221" s="2" t="s">
         <v>222</v>
       </c>
@@ -18893,7 +18912,7 @@
         <v>5255</v>
       </c>
     </row>
-    <row r="222" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A222" s="2" t="s">
         <v>223</v>
       </c>
@@ -18904,7 +18923,7 @@
         <v>5051</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A223" s="2" t="s">
         <v>224</v>
       </c>
@@ -18918,7 +18937,7 @@
         <v>5255</v>
       </c>
     </row>
-    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
       <c r="A224" s="2" t="s">
         <v>225</v>
       </c>

</xml_diff>